<commit_message>
Update outputs to fix minor issues
</commit_message>
<xml_diff>
--- a/outputs/fmtd_regression_outs_no_retal_v2.xlsx
+++ b/outputs/fmtd_regression_outs_no_retal_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisabethsilver/Documents/EEOC-AWD/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09661AFE-ECB4-EF40-A020-8A9C508B7E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00BA6DF-7918-B341-A28D-556D9E906735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="20960" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <t>0.57</t>
   </si>
   <si>
-    <t>9.98***</t>
-  </si>
-  <si>
     <t>Model 1</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>Column5</t>
+  </si>
+  <si>
+    <t>3.60*</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -483,7 +483,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -499,18 +499,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FAC4FDE-EF4E-2047-80B7-E3B42531A636}" name="Table1" displayName="Table1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FAC4FDE-EF4E-2047-80B7-E3B42531A636}" name="Table1" displayName="Table1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I13" xr:uid="{2FAC4FDE-EF4E-2047-80B7-E3B42531A636}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{F40A43D0-3EF7-ED47-8005-C9A253529069}" name="Column1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{C0BD41EC-B8BC-024A-B93D-C4B3F724206D}" name="Model 1" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{5ABC9474-2013-264A-B3DB-E6B249167D7B}" name="Column2" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{DC4EB07A-B1AD-2D42-99C0-D71E703DFBF0}" name="Model 2a" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{9A47EFDD-BE31-C947-9EC0-A046D2154C6B}" name="Column3" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{956338AB-87D8-9647-8C5D-C85CC825BEA9}" name="Model 2b" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{163B146E-52AD-7F4D-8B47-43BE2CA6A9E4}" name="Column4" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{05C4D73A-1EDA-EA48-AD98-A57E77907B3D}" name="Model 3" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{ACCC9C2A-C7E9-0040-8551-9E5B0E3894D6}" name="Column5" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F40A43D0-3EF7-ED47-8005-C9A253529069}" name="Column1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C0BD41EC-B8BC-024A-B93D-C4B3F724206D}" name="Model 1" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{5ABC9474-2013-264A-B3DB-E6B249167D7B}" name="Column2" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{DC4EB07A-B1AD-2D42-99C0-D71E703DFBF0}" name="Model 2a" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9A47EFDD-BE31-C947-9EC0-A046D2154C6B}" name="Column3" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{956338AB-87D8-9647-8C5D-C85CC825BEA9}" name="Model 2b" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{163B146E-52AD-7F4D-8B47-43BE2CA6A9E4}" name="Column4" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{05C4D73A-1EDA-EA48-AD98-A57E77907B3D}" name="Model 3" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{ACCC9C2A-C7E9-0040-8551-9E5B0E3894D6}" name="Column5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -798,7 +798,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -816,31 +816,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -848,28 +848,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="F2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="H2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
         <v>35</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>